<commit_message>
SAXS ureia mais ME, sólidos
</commit_message>
<xml_diff>
--- a/SAXS Ureia Distância intermicelar.xlsx
+++ b/SAXS Ureia Distância intermicelar.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>CTAB</t>
   </si>
@@ -45,6 +45,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,8 +77,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,15 +395,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D17"/>
+  <dimension ref="B3:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -408,8 +424,23 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H6" si="0">D5</f>
+        <v>12.491422081867965</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I6" si="1">D10</f>
+        <v>9.7112601347443377</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J6" si="2">D15</f>
+        <v>9.4483989581647911</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>100</v>
       </c>
@@ -420,8 +451,23 @@
         <f>2*PI()/C5</f>
         <v>12.491422081867965</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>200</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>10.4545512598662</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>8.2673490883941927</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="2"/>
+        <v>7.1481061515126125</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>200</v>
       </c>
@@ -429,11 +475,26 @@
         <v>0.60099999999999998</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D17" si="0">2*PI()/C6</f>
+        <f t="shared" ref="D6:D17" si="3">2*PI()/C6</f>
         <v>10.4545512598662</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>300</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>9.5780263828957111</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>7.551905417283157</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="2"/>
+        <v>6.3147591026930519</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>300</v>
       </c>
@@ -441,16 +502,16 @@
         <v>0.65600000000000003</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.5780263828957111</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>100</v>
       </c>
@@ -458,11 +519,11 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.7112601347443377</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>200</v>
       </c>
@@ -470,11 +531,11 @@
         <v>0.76</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8.2673490883941927</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>300</v>
       </c>
@@ -482,16 +543,16 @@
         <v>0.83199999999999996</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.551905417283157</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>100</v>
       </c>
@@ -499,11 +560,11 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.4483989581647911</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>200</v>
       </c>
@@ -511,7 +572,7 @@
         <v>0.879</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.1481061515126125</v>
       </c>
     </row>
@@ -523,7 +584,7 @@
         <v>0.995</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.3147591026930519</v>
       </c>
     </row>

</xml_diff>